<commit_message>
resolved issue checked and closed
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/forget password/forget_password.xlsx
+++ b/apps/features/backlog/desktop/windows/forget password/forget_password.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\forget password\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4572AFD4-9D17-4713-BC5C-1E4C49B6464F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF3825D-2051-40B6-8D10-8B7EF960A30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1668,8 +1668,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1883,7 +1883,7 @@
         <v>114</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="3"/>

</xml_diff>

<commit_message>
forget pass page check
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/forget password/forget_password.xlsx
+++ b/apps/features/backlog/desktop/windows/forget password/forget_password.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\forget password\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF3825D-2051-40B6-8D10-8B7EF960A30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4D09C9-A33B-4A76-BC2D-07B5F1EA8404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="130">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -529,6 +529,9 @@
   <si>
     <t>check after clicking the send button with javascript disabled</t>
   </si>
+  <si>
+    <t>Ref ID</t>
+  </si>
 </sst>
 </file>
 
@@ -721,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -802,11 +805,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="57">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1358,84 +1399,84 @@
   </dxfs>
   <tableStyles count="16">
     <tableStyle name="Template-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="55"/>
-      <tableStyleElement type="firstRowStripe" dxfId="54"/>
-      <tableStyleElement type="secondRowStripe" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="56"/>
+      <tableStyleElement type="firstRowStripe" dxfId="55"/>
+      <tableStyleElement type="secondRowStripe" dxfId="54"/>
     </tableStyle>
     <tableStyle name="1419-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="52"/>
-      <tableStyleElement type="firstRowStripe" dxfId="51"/>
-      <tableStyleElement type="secondRowStripe" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
+      <tableStyleElement type="firstRowStripe" dxfId="52"/>
+      <tableStyleElement type="secondRowStripe" dxfId="51"/>
     </tableStyle>
     <tableStyle name="2147-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="49"/>
-      <tableStyleElement type="firstRowStripe" dxfId="48"/>
-      <tableStyleElement type="secondRowStripe" dxfId="47"/>
+      <tableStyleElement type="headerRow" dxfId="50"/>
+      <tableStyleElement type="firstRowStripe" dxfId="49"/>
+      <tableStyleElement type="secondRowStripe" dxfId="48"/>
     </tableStyle>
     <tableStyle name="2170-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="46"/>
-      <tableStyleElement type="firstRowStripe" dxfId="45"/>
-      <tableStyleElement type="secondRowStripe" dxfId="44"/>
+      <tableStyleElement type="headerRow" dxfId="47"/>
+      <tableStyleElement type="firstRowStripe" dxfId="46"/>
+      <tableStyleElement type="secondRowStripe" dxfId="45"/>
     </tableStyle>
     <tableStyle name="2177-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="43"/>
-      <tableStyleElement type="firstRowStripe" dxfId="42"/>
-      <tableStyleElement type="secondRowStripe" dxfId="41"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="firstRowStripe" dxfId="43"/>
+      <tableStyleElement type="secondRowStripe" dxfId="42"/>
     </tableStyle>
     <tableStyle name="2253-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="40"/>
-      <tableStyleElement type="firstRowStripe" dxfId="39"/>
-      <tableStyleElement type="secondRowStripe" dxfId="38"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="secondRowStripe" dxfId="39"/>
     </tableStyle>
     <tableStyle name="2255-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="37"/>
-      <tableStyleElement type="firstRowStripe" dxfId="36"/>
-      <tableStyleElement type="secondRowStripe" dxfId="35"/>
+      <tableStyleElement type="headerRow" dxfId="38"/>
+      <tableStyleElement type="firstRowStripe" dxfId="37"/>
+      <tableStyleElement type="secondRowStripe" dxfId="36"/>
     </tableStyle>
     <tableStyle name="2274-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="secondRowStripe" dxfId="32"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="firstRowStripe" dxfId="34"/>
+      <tableStyleElement type="secondRowStripe" dxfId="33"/>
     </tableStyle>
     <tableStyle name="2277-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="31"/>
-      <tableStyleElement type="firstRowStripe" dxfId="30"/>
-      <tableStyleElement type="secondRowStripe" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="32"/>
+      <tableStyleElement type="firstRowStripe" dxfId="31"/>
+      <tableStyleElement type="secondRowStripe" dxfId="30"/>
     </tableStyle>
     <tableStyle name="2279-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="28"/>
-      <tableStyleElement type="firstRowStripe" dxfId="27"/>
-      <tableStyleElement type="secondRowStripe" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="firstRowStripe" dxfId="28"/>
+      <tableStyleElement type="secondRowStripe" dxfId="27"/>
     </tableStyle>
     <tableStyle name="2280-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0A000000}">
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="firstRowStripe" dxfId="24"/>
-      <tableStyleElement type="secondRowStripe" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="firstRowStripe" dxfId="25"/>
+      <tableStyleElement type="secondRowStripe" dxfId="24"/>
     </tableStyle>
     <tableStyle name="2283-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0B000000}">
-      <tableStyleElement type="headerRow" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="secondRowStripe" dxfId="21"/>
     </tableStyle>
     <tableStyle name="2285-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0C000000}">
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
     <tableStyle name="2287-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0D000000}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
     <tableStyle name="2292-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0E000000}">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
     <tableStyle name="2293-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0F000000}">
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1450,15 +1491,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G32" dataDxfId="7">
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:H32" dataDxfId="8">
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{9B0F1D71-8AC9-4A83-AB3B-49171C00F802}" name="Ref ID" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1665,11 +1707,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:AA990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1679,12 +1721,11 @@
     <col min="3" max="3" width="45.6640625" style="14" customWidth="1"/>
     <col min="4" max="4" width="50.6640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="45.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="16" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>127</v>
       </c>
@@ -1714,7 +1755,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1742,7 +1783,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
@@ -1758,13 +1799,15 @@
       <c r="E3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1783,8 +1826,9 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:27" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1800,13 +1844,13 @@
       <c r="E4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1825,8 +1869,9 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
-    </row>
-    <row r="5" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1842,11 +1887,11 @@
       <c r="E5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1865,8 +1910,9 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
-    </row>
-    <row r="6" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1882,11 +1928,11 @@
       <c r="E6" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1905,8 +1951,9 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
-    </row>
-    <row r="7" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" spans="1:27" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
@@ -1922,11 +1969,13 @@
       <c r="E7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>50</v>
+      <c r="F7" s="28">
+        <v>9251</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="7"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1945,8 +1994,9 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -1962,11 +2012,11 @@
       <c r="E8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1985,8 +2035,9 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
@@ -2002,11 +2053,11 @@
       <c r="E9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2025,8 +2076,9 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA9" s="4"/>
+    </row>
+    <row r="10" spans="1:27" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2042,11 +2094,11 @@
       <c r="E10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2065,8 +2117,9 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA10" s="4"/>
+    </row>
+    <row r="11" spans="1:27" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
@@ -2082,11 +2135,11 @@
       <c r="E11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -2105,8 +2158,9 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-    </row>
-    <row r="12" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>16</v>
       </c>
@@ -2122,11 +2176,11 @@
       <c r="E12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -2145,8 +2199,9 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-    </row>
-    <row r="13" spans="1:26" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
@@ -2162,11 +2217,11 @@
       <c r="E13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -2185,8 +2240,9 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
-    </row>
-    <row r="14" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
@@ -2202,11 +2258,11 @@
       <c r="E14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="9"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -2225,8 +2281,9 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
@@ -2242,11 +2299,11 @@
       <c r="E15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2265,8 +2322,9 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
-    </row>
-    <row r="16" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
@@ -2282,11 +2340,11 @@
       <c r="E16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2305,8 +2363,9 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
-    </row>
-    <row r="17" spans="1:26" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="1:27" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
@@ -2322,11 +2381,11 @@
       <c r="E17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2345,8 +2404,9 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
-    </row>
-    <row r="18" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA17" s="1"/>
+    </row>
+    <row r="18" spans="1:27" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
@@ -2362,11 +2422,11 @@
       <c r="E18" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -2385,8 +2445,9 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-    </row>
-    <row r="19" spans="1:26" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA18" s="1"/>
+    </row>
+    <row r="19" spans="1:27" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>23</v>
       </c>
@@ -2402,11 +2463,11 @@
       <c r="E19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -2425,8 +2486,9 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
-    </row>
-    <row r="20" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA19" s="1"/>
+    </row>
+    <row r="20" spans="1:27" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>24</v>
       </c>
@@ -2442,11 +2504,11 @@
       <c r="E20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="1"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2465,8 +2527,9 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-    </row>
-    <row r="21" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA20" s="1"/>
+    </row>
+    <row r="21" spans="1:27" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>25</v>
       </c>
@@ -2482,11 +2545,11 @@
       <c r="E21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2505,8 +2568,9 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-    </row>
-    <row r="22" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA21" s="1"/>
+    </row>
+    <row r="22" spans="1:27" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>26</v>
       </c>
@@ -2522,11 +2586,11 @@
       <c r="E22" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="9"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2545,8 +2609,9 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
-    </row>
-    <row r="23" spans="1:26" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA22" s="1"/>
+    </row>
+    <row r="23" spans="1:27" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>28</v>
       </c>
@@ -2562,11 +2627,11 @@
       <c r="E23" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2585,8 +2650,9 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
-    </row>
-    <row r="24" spans="1:26" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA23" s="1"/>
+    </row>
+    <row r="24" spans="1:27" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>29</v>
       </c>
@@ -2602,11 +2668,11 @@
       <c r="E24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="1"/>
+      <c r="H24" s="9"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2625,8 +2691,9 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
-    </row>
-    <row r="25" spans="1:26" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA24" s="1"/>
+    </row>
+    <row r="25" spans="1:27" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>30</v>
       </c>
@@ -2642,11 +2709,11 @@
       <c r="E25" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="9"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2665,8 +2732,9 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
-    </row>
-    <row r="26" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA25" s="1"/>
+    </row>
+    <row r="26" spans="1:27" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>31</v>
       </c>
@@ -2682,11 +2750,11 @@
       <c r="E26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -2705,8 +2773,9 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
-    </row>
-    <row r="27" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA26" s="1"/>
+    </row>
+    <row r="27" spans="1:27" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>77</v>
       </c>
@@ -2722,11 +2791,11 @@
       <c r="E27" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="9"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2745,8 +2814,9 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
-    </row>
-    <row r="28" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA27" s="1"/>
+    </row>
+    <row r="28" spans="1:27" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>82</v>
       </c>
@@ -2762,11 +2832,11 @@
       <c r="E28" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="10"/>
+      <c r="G28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="1"/>
+      <c r="H28" s="9"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2785,8 +2855,9 @@
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
-    </row>
-    <row r="29" spans="1:26" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA28" s="1"/>
+    </row>
+    <row r="29" spans="1:27" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>83</v>
       </c>
@@ -2802,11 +2873,11 @@
       <c r="E29" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="10"/>
+      <c r="G29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="1"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2825,8 +2896,9 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
-    </row>
-    <row r="30" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA29" s="1"/>
+    </row>
+    <row r="30" spans="1:27" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>86</v>
       </c>
@@ -2842,11 +2914,11 @@
       <c r="E30" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="10"/>
+      <c r="G30" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="1"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -2865,8 +2937,9 @@
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
-    </row>
-    <row r="31" spans="1:26" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA30" s="1"/>
+    </row>
+    <row r="31" spans="1:27" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>119</v>
       </c>
@@ -2882,11 +2955,11 @@
       <c r="E31" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="1"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -2905,8 +2978,9 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-    </row>
-    <row r="32" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA31" s="1"/>
+    </row>
+    <row r="32" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>126</v>
       </c>
@@ -2922,11 +2996,11 @@
       <c r="E32" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="10"/>
+      <c r="G32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="9"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2945,6 +3019,7 @@
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
@@ -29775,7 +29850,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G32" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>